<commit_message>
Se finaliza la optimización de la zona de calor
</commit_message>
<xml_diff>
--- a/02 Optimización láminas/Datos simulación.xlsx
+++ b/02 Optimización láminas/Datos simulación.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leo7s\Documents\Universidad\04 PAI\03 Proyecto\03 Repositorio\Proyecto_PAI_2021\02 Optimización láminas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1053DFF6-AFAA-4C94-ADE9-3FC4C72C0ED4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51DA96F-A11E-4F1E-8BB0-54F4B686F55C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lamina Resistencias" sheetId="1" r:id="rId1"/>
     <sheet name="Soporte Zona Calor" sheetId="3" r:id="rId2"/>
-    <sheet name="Pesos" sheetId="2" r:id="rId3"/>
+    <sheet name="Carcasa Superior" sheetId="4" r:id="rId3"/>
+    <sheet name="Pesos" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="36">
   <si>
     <t>FS MIN</t>
   </si>
@@ -126,6 +127,24 @@
   </si>
   <si>
     <t>Barra inoxidable 5/8"</t>
+  </si>
+  <si>
+    <t>0,76 mm</t>
+  </si>
+  <si>
+    <t>Tapa superior</t>
+  </si>
+  <si>
+    <t>Carcasa superior</t>
+  </si>
+  <si>
+    <t>Tapa</t>
+  </si>
+  <si>
+    <t>Laterales</t>
+  </si>
+  <si>
+    <t>Lateral</t>
   </si>
 </sst>
 </file>
@@ -216,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -251,6 +270,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,11 +1112,222 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA69FF8-915C-4C37-94CD-20911586C069}">
-  <dimension ref="B4:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C69F546-1EE7-4E5B-A643-15DC873D6E53}">
+  <dimension ref="B1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="6">
+        <v>22</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9">
+        <f>2.076</f>
+        <v>2.0760000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45.15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="E4" s="7">
+        <v>5.49</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>57.78</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>91.92</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>91.27</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1">
+        <v>89.12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.06</v>
+      </c>
+      <c r="E8" s="1">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="6">
+        <v>22</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="C19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0.67600000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>28.12</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="E20" s="7">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA69FF8-915C-4C37-94CD-20911586C069}">
+  <dimension ref="B4:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,7 +1338,7 @@
     <col min="5" max="5" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
@@ -1119,7 +1352,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1134,7 +1367,7 @@
         <v>2.4000000000000004</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1149,7 +1382,7 @@
         <v>2.141</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
@@ -1164,7 +1397,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1179,7 +1412,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1427,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
@@ -1209,7 +1442,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1224,7 +1457,7 @@
         <v>0.73199999999999998</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1239,7 +1472,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
@@ -1254,7 +1487,7 @@
         <v>1.1719999999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
@@ -1268,9 +1501,43 @@
         <f t="shared" si="0"/>
         <v>2.5939999999999999</v>
       </c>
-      <c r="F14">
-        <f>SUM(E5:E13)</f>
-        <v>8.3870000000000005</v>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <f>D16+2*D17</f>
+        <v>3.4279999999999999</v>
+      </c>
+      <c r="E15" s="2">
+        <f>D15</f>
+        <v>3.4279999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2.0760000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.67600000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>